<commit_message>
Data cleaning on circuits.xls - Corrected special characters
</commit_message>
<xml_diff>
--- a/Data xlsx/circuits.xlsx
+++ b/Data xlsx/circuits.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analysis\Formula 1\Data xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E110117A-D2B6-4FA1-A453-FF5FD469775B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A69FCBD-9862-487B-9F2F-85DF6EF921F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="349">
   <si>
     <t>circuitId</t>
   </si>
@@ -100,9 +100,6 @@
     <t>Circuit de Barcelona-Catalunya</t>
   </si>
   <si>
-    <t>MontmelÃ³</t>
-  </si>
-  <si>
     <t>Spain</t>
   </si>
   <si>
@@ -304,12 +301,6 @@
     <t>interlagos</t>
   </si>
   <si>
-    <t>AutÃ³dromo JosÃ© Carlos Pace</t>
-  </si>
-  <si>
-    <t>SÃ£o Paulo</t>
-  </si>
-  <si>
     <t>Brazil</t>
   </si>
   <si>
@@ -334,12 +325,6 @@
     <t>nurburgring</t>
   </si>
   <si>
-    <t>NÃ¼rburgring</t>
-  </si>
-  <si>
-    <t>NÃ¼rburg</t>
-  </si>
-  <si>
     <t>http://en.wikipedia.org/wiki/N%C3%BCrburgring</t>
   </si>
   <si>
@@ -403,9 +388,6 @@
     <t>galvez</t>
   </si>
   <si>
-    <t>AutÃ³dromo Juan y Oscar GÃ¡lvez</t>
-  </si>
-  <si>
     <t>Buenos Aires</t>
   </si>
   <si>
@@ -430,9 +412,6 @@
     <t>estoril</t>
   </si>
   <si>
-    <t>AutÃ³dromo do Estoril</t>
-  </si>
-  <si>
     <t>Estoril</t>
   </si>
   <si>
@@ -496,9 +475,6 @@
     <t>rodriguez</t>
   </si>
   <si>
-    <t>AutÃ³dromo Hermanos RodrÃ­guez</t>
-  </si>
-  <si>
     <t>Mexico City</t>
   </si>
   <si>
@@ -550,9 +526,6 @@
     <t>jacarepagua</t>
   </si>
   <si>
-    <t>AutÃ³dromo Internacional Nelson Piquet</t>
-  </si>
-  <si>
     <t>Rio de Janeiro</t>
   </si>
   <si>
@@ -712,9 +685,6 @@
     <t>montjuic</t>
   </si>
   <si>
-    <t>MontjuÃ¯c</t>
-  </si>
-  <si>
     <t>Barcelona</t>
   </si>
   <si>
@@ -1009,12 +979,6 @@
     <t>portimao</t>
   </si>
   <si>
-    <t>AutÃ³dromo Internacional do Algarve</t>
-  </si>
-  <si>
-    <t>PortimÃ£o</t>
-  </si>
-  <si>
     <t>http://en.wikipedia.org/wiki/Algarve_International_Circuit</t>
   </si>
   <si>
@@ -1070,6 +1034,39 @@
   </si>
   <si>
     <t>http://en.wikipedia.org/wiki/Miami_International_Autodrome</t>
+  </si>
+  <si>
+    <t>Autodromo Internacional do Algarve</t>
+  </si>
+  <si>
+    <t>Portimao</t>
+  </si>
+  <si>
+    <t>Autodromo Juan y Oscar Galvez</t>
+  </si>
+  <si>
+    <t>Nurburgring</t>
+  </si>
+  <si>
+    <t>Autodromo Joao Carlos Pace</t>
+  </si>
+  <si>
+    <t>Sao Paulo</t>
+  </si>
+  <si>
+    <t>Autodromo do Estoril</t>
+  </si>
+  <si>
+    <t>Autodromo Hermanos Rodriguez</t>
+  </si>
+  <si>
+    <t>Autodromo Internacional Nelson Piquet</t>
+  </si>
+  <si>
+    <t>Montjuic</t>
+  </si>
+  <si>
+    <t>Montmelo</t>
   </si>
 </sst>
 </file>
@@ -1931,7 +1928,7 @@
   <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2074,10 +2071,10 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
+        <v>348</v>
+      </c>
+      <c r="E5" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
       </c>
       <c r="F5">
         <v>41.57</v>
@@ -2089,7 +2086,7 @@
         <v>109</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2097,16 +2094,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
       </c>
       <c r="F6">
         <v>40.951700000000002</v>
@@ -2118,7 +2115,7 @@
         <v>130</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2126,16 +2123,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
       </c>
       <c r="F7">
         <v>43.734699999999997</v>
@@ -2147,7 +2144,7 @@
         <v>7</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2155,16 +2152,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>40</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
       </c>
       <c r="F8">
         <v>45.5</v>
@@ -2176,7 +2173,7 @@
         <v>13</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2184,16 +2181,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
         <v>44</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>45</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
       </c>
       <c r="F9">
         <v>46.864199999999997</v>
@@ -2205,7 +2202,7 @@
         <v>228</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2213,16 +2210,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
         <v>49</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>51</v>
-      </c>
-      <c r="E10" t="s">
-        <v>52</v>
       </c>
       <c r="F10">
         <v>52.078600000000002</v>
@@ -2234,7 +2231,7 @@
         <v>153</v>
       </c>
       <c r="I10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2242,16 +2239,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
         <v>54</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>55</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>56</v>
-      </c>
-      <c r="E11" t="s">
-        <v>57</v>
       </c>
       <c r="F11">
         <v>49.327800000000003</v>
@@ -2263,7 +2260,7 @@
         <v>103</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2271,16 +2268,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
         <v>59</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>61</v>
-      </c>
-      <c r="E12" t="s">
-        <v>62</v>
       </c>
       <c r="F12">
         <v>47.578899999999997</v>
@@ -2292,7 +2289,7 @@
         <v>264</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2300,16 +2297,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
         <v>64</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>65</v>
       </c>
-      <c r="D13" t="s">
-        <v>66</v>
-      </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13">
         <v>39.4589</v>
@@ -2321,7 +2318,7 @@
         <v>4</v>
       </c>
       <c r="I13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2329,16 +2326,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" t="s">
         <v>68</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>69</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>70</v>
-      </c>
-      <c r="E14" t="s">
-        <v>71</v>
       </c>
       <c r="F14">
         <v>50.437199999999997</v>
@@ -2350,7 +2347,7 @@
         <v>401</v>
       </c>
       <c r="I14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2358,16 +2355,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
         <v>73</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>74</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>75</v>
-      </c>
-      <c r="E15" t="s">
-        <v>76</v>
       </c>
       <c r="F15">
         <v>45.615600000000001</v>
@@ -2379,7 +2376,7 @@
         <v>162</v>
       </c>
       <c r="I15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2387,16 +2384,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
         <v>78</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>79</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>80</v>
-      </c>
-      <c r="E16" t="s">
-        <v>81</v>
       </c>
       <c r="F16">
         <v>1.2914000000000001</v>
@@ -2408,7 +2405,7 @@
         <v>18</v>
       </c>
       <c r="I16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2416,16 +2413,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" t="s">
         <v>83</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>84</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>85</v>
-      </c>
-      <c r="E17" t="s">
-        <v>86</v>
       </c>
       <c r="F17">
         <v>35.371699999999997</v>
@@ -2437,7 +2434,7 @@
         <v>583</v>
       </c>
       <c r="I17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2445,16 +2442,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" t="s">
         <v>88</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>89</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>90</v>
-      </c>
-      <c r="E18" t="s">
-        <v>91</v>
       </c>
       <c r="F18">
         <v>31.338899999999999</v>
@@ -2466,7 +2463,7 @@
         <v>5</v>
       </c>
       <c r="I18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2474,16 +2471,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" t="s">
+        <v>342</v>
+      </c>
+      <c r="D19" t="s">
+        <v>343</v>
+      </c>
+      <c r="E19" t="s">
         <v>93</v>
-      </c>
-      <c r="C19" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" t="s">
-        <v>96</v>
       </c>
       <c r="F19">
         <v>-23.703600000000002</v>
@@ -2495,7 +2492,7 @@
         <v>785</v>
       </c>
       <c r="I19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2503,16 +2500,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" t="s">
         <v>98</v>
-      </c>
-      <c r="C20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" t="s">
-        <v>101</v>
       </c>
       <c r="F20">
         <v>39.795000000000002</v>
@@ -2524,7 +2521,7 @@
         <v>223</v>
       </c>
       <c r="I20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2532,16 +2529,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>341</v>
       </c>
       <c r="D21" t="s">
-        <v>105</v>
+        <v>341</v>
       </c>
       <c r="E21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F21">
         <v>50.335599999999999</v>
@@ -2553,7 +2550,7 @@
         <v>578</v>
       </c>
       <c r="I21" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2561,16 +2558,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D22" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F22">
         <v>44.343899999999998</v>
@@ -2582,7 +2579,7 @@
         <v>37</v>
       </c>
       <c r="I22" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2590,16 +2587,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C23" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F23">
         <v>34.8431</v>
@@ -2611,7 +2608,7 @@
         <v>45</v>
       </c>
       <c r="I23" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2619,16 +2616,16 @@
         <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E24" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F24">
         <v>36.114699999999999</v>
@@ -2637,10 +2634,10 @@
         <v>-115.173</v>
       </c>
       <c r="H24" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I24" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2648,16 +2645,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F25">
         <v>24.467199999999998</v>
@@ -2669,7 +2666,7 @@
         <v>3</v>
       </c>
       <c r="I25" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2677,16 +2674,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s">
-        <v>127</v>
+        <v>340</v>
       </c>
       <c r="D26" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E26" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F26">
         <v>-34.694299999999998</v>
@@ -2698,7 +2695,7 @@
         <v>8</v>
       </c>
       <c r="I26" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2706,16 +2703,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C27" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D27" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F27">
         <v>36.708300000000001</v>
@@ -2727,7 +2724,7 @@
         <v>37</v>
       </c>
       <c r="I27" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2735,16 +2732,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C28" t="s">
-        <v>136</v>
+        <v>344</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F28">
         <v>38.750599999999999</v>
@@ -2756,7 +2753,7 @@
         <v>130</v>
       </c>
       <c r="I28" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2764,16 +2761,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D29" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F29">
         <v>34.914999999999999</v>
@@ -2785,7 +2782,7 @@
         <v>266</v>
       </c>
       <c r="I29" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2793,13 +2790,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C30" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D30" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -2814,7 +2811,7 @@
         <v>58</v>
       </c>
       <c r="I30" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2822,16 +2819,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C31" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D31" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E31" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F31">
         <v>-25.9894</v>
@@ -2843,7 +2840,7 @@
         <v>1460</v>
       </c>
       <c r="I31" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2851,16 +2848,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C32" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D32" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F32">
         <v>52.830599999999997</v>
@@ -2872,7 +2869,7 @@
         <v>88</v>
       </c>
       <c r="I32" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2880,16 +2877,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C33" t="s">
-        <v>158</v>
+        <v>345</v>
       </c>
       <c r="D33" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E33" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F33">
         <v>19.404199999999999</v>
@@ -2901,7 +2898,7 @@
         <v>2227</v>
       </c>
       <c r="I33" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2909,16 +2906,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D34" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E34" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F34">
         <v>33.447899999999997</v>
@@ -2930,7 +2927,7 @@
         <v>345</v>
       </c>
       <c r="I34" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2938,16 +2935,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C35" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D35" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F35">
         <v>43.250599999999999</v>
@@ -2959,7 +2956,7 @@
         <v>432</v>
       </c>
       <c r="I35" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2967,16 +2964,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C36" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D36" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="E36" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="F36">
         <v>34.7333</v>
@@ -2988,7 +2985,7 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2996,16 +2993,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C37" t="s">
-        <v>176</v>
+        <v>346</v>
       </c>
       <c r="D37" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="E37" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F37">
         <v>-22.9756</v>
@@ -3017,7 +3014,7 @@
         <v>1126</v>
       </c>
       <c r="I37" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3025,16 +3022,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C38" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D38" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="E38" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F38">
         <v>42.329799999999999</v>
@@ -3046,7 +3043,7 @@
         <v>177</v>
       </c>
       <c r="I38" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3054,16 +3051,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C39" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D39" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F39">
         <v>51.356900000000003</v>
@@ -3075,7 +3072,7 @@
         <v>145</v>
       </c>
       <c r="I39" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3083,16 +3080,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C40" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="D40" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E40" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F40">
         <v>52.388800000000003</v>
@@ -3104,7 +3101,7 @@
         <v>6</v>
       </c>
       <c r="I40" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3112,16 +3109,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C41" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D41" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="E41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F41">
         <v>50.989400000000003</v>
@@ -3133,7 +3130,7 @@
         <v>36</v>
       </c>
       <c r="I41" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3141,16 +3138,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C42" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D42" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F42">
         <v>47.362499999999997</v>
@@ -3162,7 +3159,7 @@
         <v>484</v>
       </c>
       <c r="I42" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3170,16 +3167,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C43" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D43" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E43" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F43">
         <v>32.7774</v>
@@ -3191,7 +3188,7 @@
         <v>139</v>
       </c>
       <c r="I43" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3199,16 +3196,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C44" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="D44" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="E44" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F44">
         <v>33.765099999999997</v>
@@ -3220,7 +3217,7 @@
         <v>12</v>
       </c>
       <c r="I44" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3228,16 +3225,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C45" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D45" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E45" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F45">
         <v>36.116199999999999</v>
@@ -3249,7 +3246,7 @@
         <v>639</v>
       </c>
       <c r="I45" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3257,16 +3254,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C46" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D46" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F46">
         <v>40.617100000000001</v>
@@ -3278,7 +3275,7 @@
         <v>609</v>
       </c>
       <c r="I46" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3286,16 +3283,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C47" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D47" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="E47" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F47">
         <v>42.3369</v>
@@ -3307,7 +3304,7 @@
         <v>485</v>
       </c>
       <c r="I47" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3315,16 +3312,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C48" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D48" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E48" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="F48">
         <v>57.265300000000003</v>
@@ -3336,7 +3333,7 @@
         <v>153</v>
       </c>
       <c r="I48" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3344,16 +3341,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C49" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="D49" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="E49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F49">
         <v>44.048099999999998</v>
@@ -3365,7 +3362,7 @@
         <v>332</v>
       </c>
       <c r="I49" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -3373,16 +3370,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C50" t="s">
-        <v>230</v>
+        <v>347</v>
       </c>
       <c r="D50" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F50">
         <v>41.366399999999999</v>
@@ -3394,7 +3391,7 @@
         <v>79</v>
       </c>
       <c r="I50" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -3402,16 +3399,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C51" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="D51" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="E51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F51">
         <v>50.621099999999998</v>
@@ -3423,7 +3420,7 @@
         <v>139</v>
       </c>
       <c r="I51" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3431,16 +3428,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C52" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D52" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="E52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F52">
         <v>45.747199999999999</v>
@@ -3452,7 +3449,7 @@
         <v>790</v>
       </c>
       <c r="I52" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3460,16 +3457,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C53" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D53" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="E53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F53">
         <v>46.1877</v>
@@ -3481,7 +3478,7 @@
         <v>214</v>
       </c>
       <c r="I53" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -3489,16 +3486,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C54" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="D54" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="E54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F54">
         <v>49.330599999999997</v>
@@ -3510,7 +3507,7 @@
         <v>81</v>
       </c>
       <c r="I54" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -3518,16 +3515,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C55" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D55" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="E55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F55">
         <v>47.95</v>
@@ -3539,7 +3536,7 @@
         <v>67</v>
       </c>
       <c r="I55" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3547,16 +3544,16 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="C56" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="D56" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="E56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F56">
         <v>49.254199999999997</v>
@@ -3568,7 +3565,7 @@
         <v>88</v>
       </c>
       <c r="I56" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3576,16 +3573,16 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C57" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="D57" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="E57" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F57">
         <v>-33.0486</v>
@@ -3597,7 +3594,7 @@
         <v>15</v>
       </c>
       <c r="I57" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3605,16 +3602,16 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C58" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="D58" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="E58" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="F58">
         <v>47.203899999999997</v>
@@ -3626,7 +3623,7 @@
         <v>676</v>
       </c>
       <c r="I58" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3634,16 +3631,16 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="C59" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="D59" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="E59" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F59">
         <v>53.476900000000001</v>
@@ -3655,7 +3652,7 @@
         <v>20</v>
       </c>
       <c r="I59" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3663,16 +3660,16 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C60" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D60" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="E60" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F60">
         <v>41.170499999999997</v>
@@ -3684,7 +3681,7 @@
         <v>28</v>
       </c>
       <c r="I60" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3692,16 +3689,16 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="C61" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="D61" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="E61" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F61">
         <v>33.936999999999998</v>
@@ -3713,7 +3710,7 @@
         <v>470</v>
       </c>
       <c r="I61" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3721,16 +3718,16 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C62" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D62" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="E62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F62">
         <v>52.480600000000003</v>
@@ -3742,7 +3739,7 @@
         <v>53</v>
       </c>
       <c r="I62" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3750,16 +3747,16 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C63" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D63" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="E63" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F63">
         <v>38.719700000000003</v>
@@ -3771,7 +3768,7 @@
         <v>158</v>
       </c>
       <c r="I63" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3779,16 +3776,16 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C64" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="D64" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="E64" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F64">
         <v>27.454699999999999</v>
@@ -3800,7 +3797,7 @@
         <v>18</v>
       </c>
       <c r="I64" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3808,16 +3805,16 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="C65" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="D65" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="E65" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="F65">
         <v>33.578600000000002</v>
@@ -3829,7 +3826,7 @@
         <v>19</v>
       </c>
       <c r="I65" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3837,16 +3834,16 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="C66" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D66" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="E66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F66">
         <v>42.475000000000001</v>
@@ -3858,7 +3855,7 @@
         <v>129</v>
       </c>
       <c r="I66" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3866,16 +3863,16 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="C67" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D67" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="E67" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="F67">
         <v>46.9589</v>
@@ -3887,7 +3884,7 @@
         <v>551</v>
       </c>
       <c r="I67" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3895,16 +3892,16 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="C68" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="D68" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F68">
         <v>41.390300000000003</v>
@@ -3916,7 +3913,7 @@
         <v>85</v>
       </c>
       <c r="I68" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3924,16 +3921,16 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="C69" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="D69" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="E69" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="F69">
         <v>28.348700000000001</v>
@@ -3945,7 +3942,7 @@
         <v>194</v>
       </c>
       <c r="I69" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3953,16 +3950,16 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="C70" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="D70" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="E70" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F70">
         <v>30.1328</v>
@@ -3974,7 +3971,7 @@
         <v>161</v>
       </c>
       <c r="I70" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3982,16 +3979,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="C71" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="D71" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="E71" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="F71">
         <v>47.219700000000003</v>
@@ -4003,7 +4000,7 @@
         <v>678</v>
       </c>
       <c r="I71" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -4011,16 +4008,16 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C72" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="D72" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="E72" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="F72">
         <v>43.405700000000003</v>
@@ -4032,7 +4029,7 @@
         <v>2</v>
       </c>
       <c r="I72" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -4040,16 +4037,16 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="C73" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="D73" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="E73" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="F73">
         <v>40.372500000000002</v>
@@ -4061,7 +4058,7 @@
         <v>-7</v>
       </c>
       <c r="I73" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -4069,16 +4066,16 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="C74" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="D74" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="E74" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F74">
         <v>37.226999999999997</v>
@@ -4090,7 +4087,7 @@
         <v>108</v>
       </c>
       <c r="I74" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -4098,16 +4095,16 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="C75" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="D75" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="E75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F75">
         <v>43.997500000000002</v>
@@ -4119,7 +4116,7 @@
         <v>255</v>
       </c>
       <c r="I75" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -4127,16 +4124,16 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="C76" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="D76" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="E76" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="F76">
         <v>21.631900000000002</v>
@@ -4148,7 +4145,7 @@
         <v>15</v>
       </c>
       <c r="I76" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -4156,16 +4153,16 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="C77" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="D77" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="E77" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="F77">
         <v>25.49</v>
@@ -4174,10 +4171,10 @@
         <v>51.4542</v>
       </c>
       <c r="H77" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I77" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -4185,16 +4182,16 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="C78" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="D78" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="E78" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F78">
         <v>25.958100000000002</v>
@@ -4203,10 +4200,10 @@
         <v>-80.238900000000001</v>
       </c>
       <c r="H78" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I78" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>